<commit_message>
Updated excel with 10 job applications
</commit_message>
<xml_diff>
--- a/Applications_Internship.xlsx
+++ b/Applications_Internship.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY_work\Internship-Application-Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CCFF9B-53B6-4E39-B1A3-04C9BD88777F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0B73D9-B34E-4ACC-B8D9-96FAFEA5E2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>SL.NO.</t>
   </si>
@@ -104,17 +104,86 @@
     <t>Accepted:</t>
   </si>
   <si>
-    <t>Awaiting Resonse:</t>
-  </si>
-  <si>
     <t>Declined:</t>
+  </si>
+  <si>
+    <t>Adobe</t>
+  </si>
+  <si>
+    <t>https://adobe.wd5.myworkdayjobs.com/en-US/external_experienced/userHome</t>
+  </si>
+  <si>
+    <t>Awaiting Resonse/In Process:</t>
+  </si>
+  <si>
+    <t>Applied - In Process</t>
+  </si>
+  <si>
+    <t>https://sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=25235&amp;siteid=5359#Applications</t>
+  </si>
+  <si>
+    <t>Synopsys</t>
+  </si>
+  <si>
+    <t>Applied</t>
+  </si>
+  <si>
+    <t>CareSource</t>
+  </si>
+  <si>
+    <t>Thomson Reuters</t>
+  </si>
+  <si>
+    <t>https://caresource.wd1.myworkdayjobs.com/en-US/CareSource/userHome</t>
+  </si>
+  <si>
+    <t>Applied - In Progress</t>
+  </si>
+  <si>
+    <t>https://thomsonreuters.wd5.myworkdayjobs.com/en-US/External_Career_Site/userHome</t>
+  </si>
+  <si>
+    <t>https://gwu.joinhandshake.com/stu/jobs/8467625?utm_source=activity_mailer&amp;utm_medium=email&amp;utm_campaign=notification_email</t>
+  </si>
+  <si>
+    <t>ADP, Inc</t>
+  </si>
+  <si>
+    <t>https://career41.sapsf.com/portalcareer?_s.crb=gKna3uvG6%252fwdQK0FaLbxPAsGSldA78puRfwb0idfmeA%253d</t>
+  </si>
+  <si>
+    <t>Qorvo</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>2 roles</t>
+  </si>
+  <si>
+    <t>https://careers-cnhind.icims.com/jobs/25070/data-engineer-intern/job?mode=submit_apply</t>
+  </si>
+  <si>
+    <t>CNH Industria</t>
+  </si>
+  <si>
+    <t>Samsung Research America</t>
+  </si>
+  <si>
+    <t>https://gwu.joinhandshake.com/stu/jobs/8462736?utm_source=activity_mailer&amp;utm_medium=email&amp;utm_campaign=notification_email</t>
+  </si>
+  <si>
+    <t>https://dowjones.wd1.myworkdayjobs.com/en-US/Dow_Jones_Career/userHome</t>
+  </si>
+  <si>
+    <t>Dow Jones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +204,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF494949"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="7">
@@ -184,10 +273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -198,8 +288,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,14 +582,16 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="73.88671875" customWidth="1"/>
+    <col min="3" max="3" width="85.5546875" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -509,6 +607,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -517,7 +618,7 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -528,6 +629,15 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
@@ -539,6 +649,15 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
@@ -549,6 +668,15 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -559,6 +687,15 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -570,6 +707,15 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
@@ -580,6 +726,18 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -590,15 +748,42 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>11</v>
@@ -623,15 +808,15 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H14" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="5"/>
@@ -651,8 +836,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5EC48A9C-C385-4181-A514-709324F3F0FD}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{48504C85-E833-4A0A-A9DB-4D15C3A89B68}"/>
+    <hyperlink ref="C4" r:id="rId3" location="Applications" xr:uid="{845105A1-1E58-4DFA-A08C-66D7F43731CC}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{9085AAA3-9F7F-4493-9F68-6D79EFB5EAFC}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{E74AB902-733F-45EE-AFB6-04F6FD1E1B49}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{DAC3EC1A-2856-4BC2-9D86-99659337A3F8}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{48618093-0F4F-46BA-94C1-D7C2BF3D9674}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{92F8B0A9-F758-48AA-B78E-C699358F8D3C}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{D77FED68-5F2D-4CCD-83BF-EA92260AA42E}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{D163B111-F9D6-487B-9B73-65864C2C8F91}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;8&amp;K000000 Internal</oddFooter>
   </headerFooter>

</xml_diff>